<commit_message>
Edit and Delete Foreign Posts tests added
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.UI.Tests/DataDrivenTests/LoginUserData.xlsx
+++ b/Blog-Skeleton/Blog.UI.Tests/DataDrivenTests/LoginUserData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Key</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>123456</t>
+  </si>
+  <si>
+    <t>LoginForeinUserData</t>
+  </si>
+  <si>
+    <t>aaa@abv.bg</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -493,14 +499,26 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="evitta15@mail.bg"/>
     <hyperlink ref="B5" r:id="rId2"/>
     <hyperlink ref="B6" r:id="rId3"/>
     <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Manage Account Tests are ready. LogOff navigtion test added
</commit_message>
<xml_diff>
--- a/Blog-Skeleton/Blog.UI.Tests/DataDrivenTests/LoginUserData.xlsx
+++ b/Blog-Skeleton/Blog.UI.Tests/DataDrivenTests/LoginUserData.xlsx
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -510,6 +510,9 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="evitta15@mail.bg"/>

</xml_diff>